<commit_message>
add verify by email and clean code
</commit_message>
<xml_diff>
--- a/DemoHelloPayTest/data/data.xlsx
+++ b/DemoHelloPayTest/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="UserInfo" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>907838455</t>
   </si>
   <si>
-    <t>957748699</t>
-  </si>
-  <si>
     <t>duongvu@chotot.vn</t>
   </si>
   <si>
@@ -116,7 +113,10 @@
     <t>10</t>
   </si>
   <si>
-    <t>duongvu1212@gmail.com</t>
+    <t>testforever11111@gmail.com</t>
+  </si>
+  <si>
+    <t>957748600</t>
   </si>
 </sst>
 </file>
@@ -166,13 +166,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -454,7 +455,7 @@
   <dimension ref="A1:G1048572"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -501,7 +502,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -516,7 +517,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -533,7 +534,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -552,7 +553,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -569,11 +570,11 @@
         <v>12</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -590,13 +591,13 @@
         <v>12</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -613,13 +614,13 @@
         <v>12</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -636,13 +637,13 @@
         <v>15</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -659,13 +660,13 @@
         <v>12</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -679,16 +680,16 @@
         <v>11</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>29</v>
+      <c r="E11" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8492,7 +8493,6 @@
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1"/>
     <hyperlink ref="E8" r:id="rId2"/>
-    <hyperlink ref="E11" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>